<commit_message>
simplify project to use custom fields
</commit_message>
<xml_diff>
--- a/datasets/lookup_data.xlsx
+++ b/datasets/lookup_data.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Programming\git_repos\weather-analytics-api-example\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33143E77-2927-4C0F-A7C2-435BA7F5239B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B9E041-A216-415E-A832-51E95FA82062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="time_period" sheetId="1" r:id="rId1"/>
+    <sheet name="filter_by" sheetId="2" r:id="rId1"/>
+    <sheet name="time_period" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>index</t>
   </si>
@@ -78,6 +66,30 @@
   </si>
   <si>
     <t>2015-12-01</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>quarter</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>start_of_year</t>
+  </si>
+  <si>
+    <t>start_of_quarter</t>
+  </si>
+  <si>
+    <t>start_of_month</t>
   </si>
 </sst>
 </file>
@@ -435,13 +447,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3BE2B7-5737-4B70-B097-653BFEACBFD6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>